<commit_message>
desactiver et activer les comptes utilisateur
</commit_message>
<xml_diff>
--- a/Formations.xlsx
+++ b/Formations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Titre de la formation</t>
   </si>
@@ -26,31 +26,70 @@
     <t>Nombre d'étudiants inscrits</t>
   </si>
   <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Formation sur les bases de données SQL</t>
+    <t>f</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>17-07-2024</t>
+  </si>
+  <si>
+    <t>ert</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>20-07-2024</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>ffffffffff</t>
+  </si>
+  <si>
+    <t>13-07-2024</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>11-07-2024</t>
+  </si>
+  <si>
+    <t>df</t>
   </si>
   <si>
     <t>26-07-2024</t>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Formation sur le langage Python</t>
+    <t>angularrr</t>
+  </si>
+  <si>
+    <t>fdgfnfg</t>
+  </si>
+  <si>
+    <t>06-07-2024</t>
+  </si>
+  <si>
+    <t>dzfdsfds</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
   <si>
     <t>02-08-2024</t>
   </si>
   <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>Formation sur le framework Angular</t>
-  </si>
-  <si>
-    <t>25-07-2024</t>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>descFormation</t>
+  </si>
+  <si>
+    <t>07-08-2024</t>
   </si>
 </sst>
 </file>
@@ -95,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -126,7 +165,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -154,6 +193,76 @@
         <v>12</v>
       </c>
       <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D9" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>